<commit_message>
Device recall update (#197)
* Device Recall updates.

* Device Recall updates.
</commit_message>
<xml_diff>
--- a/static/fields/devicerecall_reference.xlsx
+++ b/static/fields/devicerecall_reference.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CBD78A-FA93-D841-953B-9B7D99C8B603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="7000" windowWidth="32820" windowHeight="18080" tabRatio="500"/>
+    <workbookView xWindow="38480" yWindow="460" windowWidth="38200" windowHeight="19800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_recali_fields" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t>Field Name</t>
   </si>
@@ -130,11 +136,122 @@
   <si>
     <t>If 510(k) or PMA numbers are not applicable to the device recalled, the recall may contain other regulatory descriptions, such as exempt.</t>
   </si>
+  <si>
+    <t>event_date_initiated</t>
+  </si>
+  <si>
+    <t>event_date_created</t>
+  </si>
+  <si>
+    <t>event_date_posted</t>
+  </si>
+  <si>
+    <t>Date that the firm first began notifying the public or their consignees of the recall.</t>
+  </si>
+  <si>
+    <t>Date on which the recall record was created in the FDA database.</t>
+  </si>
+  <si>
+    <t>Indicates the date FDA classified the recall, but it does not necessarily mean that the recall is new.</t>
+  </si>
+  <si>
+    <t>recall_status</t>
+  </si>
+  <si>
+    <t>recalling_firm</t>
+  </si>
+  <si>
+    <t>Current status of the recall. A record in the database is created when a firm initiates a correction or removal action.  The record is updated if the FDA identifies a violation and classifies the action as a recall, and it is updated for a final time when the recall is terminated.</t>
+  </si>
+  <si>
+    <t>The firm that initiates a recall or, in the case of an FDA requested recall or FDA mandated recall, the firm that has primary responsibility for the manufacture and (or) marketing of the product to be recalled. This field may also include the firm's full address (normally in case of international addresses)</t>
+  </si>
+  <si>
+    <t>address_1</t>
+  </si>
+  <si>
+    <t>address_2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>additional_info_contact</t>
+  </si>
+  <si>
+    <t>reason_for_recall</t>
+  </si>
+  <si>
+    <t>Street address (Line 1) of the Recalling Firm, if available.</t>
+  </si>
+  <si>
+    <t>Street address (Line 2) of the Recalling Firm, if available.</t>
+  </si>
+  <si>
+    <t>City of the Recalling Firm, if available.</t>
+  </si>
+  <si>
+    <t>US state of the Recalling Firm, if available.</t>
+  </si>
+  <si>
+    <t>ZIP or postal code of the Recalling Firm, if available.</t>
+  </si>
+  <si>
+    <t>Country of the Recalling Firm, if available.</t>
+  </si>
+  <si>
+    <t>Contact information of the party that can be used to request additional information about the recall.</t>
+  </si>
+  <si>
+    <t>Information describing how the product is defective and violates the FD&amp;C Act or related statutes.</t>
+  </si>
+  <si>
+    <t>product_description</t>
+  </si>
+  <si>
+    <t>Brief description of the product being recalled.</t>
+  </si>
+  <si>
+    <t>code_info</t>
+  </si>
+  <si>
+    <t>A list of all lot and/or serial numbers, product numbers, packer or manufacturer numbers, sell or use by dates, etc., which appear on the product or its labeling.</t>
+  </si>
+  <si>
+    <t>product_quantity</t>
+  </si>
+  <si>
+    <t>The amount of defective product subject to recall.</t>
+  </si>
+  <si>
+    <t>distribution_pattern</t>
+  </si>
+  <si>
+    <t>General area of initial distribution such as, “Distributors in 6 states: NY, VA, TX, GA, FL and MA; the Virgin Islands; Canada and Japan”. The term “nationwide” is defined to mean the fifty states or a significant portion.  Note that subsequent distribution by the consignees to other parties may not be included.</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Action taken as part of the recall.</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -474,7 +591,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -503,6 +620,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="281">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -789,6 +907,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1113,26 +1239,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="118.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1146,184 +1272,395 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="7"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
-      <c r="B7" s="4" t="s">
+    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="90">
-      <c r="B8" s="4" t="s">
+    <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="4" t="s">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="135">
-      <c r="A10" s="3" t="s">
+    <row r="28" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45">
-      <c r="A11" s="3" t="s">
+    <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60">
-      <c r="A13" s="3" t="s">
+    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45">
-      <c r="A15" s="3" t="s">
+    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="21" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="36" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Added `cfres_id` field to the Device Recalls dataset: fixes https://github.com/FDA/openfda/issues/178
</commit_message>
<xml_diff>
--- a/static/fields/devicerecall_reference.xlsx
+++ b/static/fields/devicerecall_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CBD78A-FA93-D841-953B-9B7D99C8B603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC0FC27-844A-E746-81CD-34D280D7133E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="460" windowWidth="38200" windowHeight="19800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="500" windowWidth="38200" windowHeight="19800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_recali_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Field Name</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>cfres_id</t>
+  </si>
+  <si>
+    <t>cfRes internal recall identifier</t>
   </si>
 </sst>
 </file>
@@ -1243,10 +1249,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,385 +1281,397 @@
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>41</v>
+        <v>69</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D9" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>52</v>
+      <c r="D10" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
-      <c r="B15" s="10" t="s">
-        <v>49</v>
+      <c r="B15" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="10" t="s">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="10" t="s">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B26" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="C28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="5" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>